<commit_message>
Update ToDo.xlsx with latest changes
The ToDo.xlsx file was modified. Details of the changes within the Excel file are not specified in the diff.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C402300-8033-4ED4-9A42-7FA77F7413DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A657C9F-2DF4-4047-8D91-86D364E28D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$49</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$52</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>تسک</t>
   </si>
@@ -103,18 +103,12 @@
     <t>توضيحات</t>
   </si>
   <si>
-    <t xml:space="preserve">اضافه کردن چتباکس بصورت جنرال ( یک آواتار خوشگل که همیشه معلقه و در دسترس) </t>
-  </si>
-  <si>
     <t>عضويت</t>
   </si>
   <si>
     <t>چت باکس</t>
   </si>
   <si>
-    <t>محیط حاظر باید همیشه بعنوان کانتکست بهش تزریق بشه آپشن برای تعیین ایجنت داشته باشه / همینطور قابلیت ویندو / باگها</t>
-  </si>
-  <si>
     <t>قابليت آپدیت خود AppEnd</t>
   </si>
   <si>
@@ -299,6 +293,15 @@
   </si>
   <si>
     <t>دسترسی روی فیلد</t>
+  </si>
+  <si>
+    <t>تکمیل امکانات چتباکس</t>
+  </si>
+  <si>
+    <t>ابزارها و ..... - تزریق کانتکست</t>
+  </si>
+  <si>
+    <t>تغییر عملیات کش به یک سیستم بهتر</t>
   </si>
 </sst>
 </file>
@@ -702,11 +705,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -736,21 +739,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="9">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -758,29 +761,21 @@
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="9">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
     <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -791,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -805,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="13">
         <v>0.5</v>
@@ -823,13 +818,13 @@
     </row>
     <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -843,13 +838,13 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2">
         <v>0.5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -857,36 +852,36 @@
         <v>6</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="15">
         <v>3</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="16">
         <v>1</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="9">
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
@@ -897,19 +892,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="9">
         <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="2">
         <v>0.2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -919,53 +914,53 @@
     </row>
     <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="C23" s="9">
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="9">
         <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="10">
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E27" s="6">
         <v>0.5</v>
@@ -973,16 +968,16 @@
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="10">
         <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E28" s="6">
         <v>0.5</v>
@@ -995,22 +990,22 @@
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="9">
         <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E30" s="2">
         <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -1018,19 +1013,19 @@
     </row>
     <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C31" s="9">
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
@@ -1038,19 +1033,19 @@
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32" s="9">
         <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E32" s="2">
         <v>0.1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G32"/>
       <c r="H32"/>
@@ -1058,184 +1053,148 @@
     </row>
     <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="9">
         <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E33" s="2">
         <v>0.1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
     </row>
+    <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+    </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="9">
-        <v>20</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="9">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="2">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C37" s="9">
         <v>20</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E37" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C38" s="9">
         <v>20</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E38" s="2">
         <v>2</v>
       </c>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
     </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C39" s="9">
         <v>20</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E39" s="2">
-        <v>3</v>
-      </c>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="9">
+        <v>20</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2</v>
+      </c>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
     </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C41" s="9">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E41" s="2">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
     </row>
-    <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" s="9">
-        <v>7</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-    </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C43" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E43" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C44" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E44" s="2">
         <v>0.3</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="G44"/>
       <c r="H44"/>
@@ -1243,19 +1202,19 @@
     </row>
     <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C45" s="9">
         <v>7</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E45" s="2">
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G45"/>
       <c r="H45"/>
@@ -1263,19 +1222,22 @@
     </row>
     <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C46" s="9">
         <v>7</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E46" s="2">
-        <v>5</v>
+        <v>0.3</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G46"/>
       <c r="H46"/>
@@ -1283,22 +1245,22 @@
     </row>
     <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C47" s="9">
         <v>7</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E47" s="2">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G47"/>
       <c r="H47"/>
@@ -1306,22 +1268,19 @@
     </row>
     <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C48" s="9">
         <v>7</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E48" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G48"/>
       <c r="H48"/>
@@ -1329,36 +1288,65 @@
     </row>
     <row r="49" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="9">
+        <v>7</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="9">
-        <v>50</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E49" s="2">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
     </row>
+    <row r="50" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="9">
+        <v>7</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="2">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+    </row>
     <row r="51" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C51" s="9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E51" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G51"/>
       <c r="H51"/>
@@ -1366,43 +1354,80 @@
     </row>
     <row r="52" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C52" s="9">
+        <v>50</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="2">
+        <v>3</v>
+      </c>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+    </row>
+    <row r="54" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="9">
+        <v>15</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="2">
         <v>1</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52" s="2">
+      <c r="F54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55" s="9">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="2">
         <v>0.5</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G52"/>
-    </row>
-    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G53"/>
-    </row>
-    <row r="54" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E54" s="7">
-        <f>SUM(E7:E53)</f>
-        <v>42.3</v>
-      </c>
-      <c r="G54"/>
-    </row>
-    <row r="55" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G56"/>
     </row>
     <row r="57" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="7">
+        <f>SUM(E7:E56)</f>
+        <v>42.8</v>
+      </c>
       <c r="G57"/>
     </row>
+    <row r="58" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G60"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1425,40 +1450,40 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance caching and invalidation for DbDialog & DynaCode
- Added thread-safe caching for DbDialog and DynaCodeSettings using ConcurrentDictionary.
- Implemented cache invalidation on file changes and code refresh.
- Cached type resolution in DynaCodeMapping for performance.
- Renamed AppEndUser context cache key for clarity.
- Updated Zzz.AppEndProxy.settings.json to disable PingMe caching.
- Consolidated using statements and made minor code cleanups.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A657C9F-2DF4-4047-8D91-86D364E28D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826A00A-8EA5-45D7-8E23-2416B5B8C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$52</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$52</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
   <si>
     <t>تسک</t>
   </si>
@@ -301,7 +301,10 @@
     <t>ابزارها و ..... - تزریق کانتکست</t>
   </si>
   <si>
-    <t>تغییر عملیات کش به یک سیستم بهتر</t>
+    <t>تغییر سیستم ترجمه ها</t>
+  </si>
+  <si>
+    <t>بهینه سازی بخش عبارت ها</t>
   </si>
 </sst>
 </file>
@@ -1080,6 +1083,9 @@
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>

</xml_diff>

<commit_message>
Revert "Enhance caching and invalidation for DbDialog & DynaCode"
This reverts commit 35a80ec28c2b5533c3949bd52425f5dad611d23e.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826A00A-8EA5-45D7-8E23-2416B5B8C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A657C9F-2DF4-4047-8D91-86D364E28D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$52</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$52</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>تسک</t>
   </si>
@@ -301,10 +301,7 @@
     <t>ابزارها و ..... - تزریق کانتکست</t>
   </si>
   <si>
-    <t>تغییر سیستم ترجمه ها</t>
-  </si>
-  <si>
-    <t>بهینه سازی بخش عبارت ها</t>
+    <t>تغییر عملیات کش به یک سیستم بهتر</t>
   </si>
 </sst>
 </file>
@@ -1083,9 +1080,6 @@
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>

</xml_diff>

<commit_message>
Add custom scrollbars and responsive layout to dev guide
Custom scrollbars for .dev-guide content and nav were added for both Firefox and WebKit browsers, providing a thinner, semi-transparent appearance. The navigation sidebar now has a fixed width and 100% width styling. A media query improves the layout on large screens by allocating 220px to the sidebar and the remaining space to the main content. ToDo.xlsx was also updated.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584F745D-4911-4CA1-AD09-966649BB6EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7819C063-EEC3-475A-BE78-A2E4E6BE2370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$41</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$39</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>تسک</t>
   </si>
@@ -215,12 +215,6 @@
   </si>
   <si>
     <t>ذخيره بازيابی</t>
-  </si>
-  <si>
-    <t>پشتیبانی از لانگرانینگ تسکس</t>
-  </si>
-  <si>
-    <t>انجين</t>
   </si>
   <si>
     <t>اعتبارسنجی</t>
@@ -681,11 +675,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -718,18 +712,18 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="9">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -737,13 +731,13 @@
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="9">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -770,189 +764,215 @@
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="9">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="12">
+        <v>3</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="13">
         <v>1</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C9" s="9">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="12">
-        <v>3</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="13">
-        <v>1</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="C10" s="9">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="9">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="9">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="10">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="10">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="9">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="D18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="9">
         <v>4</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="9">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="10">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="10">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
+      <c r="F19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
     </row>
     <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E20" s="2">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
@@ -960,7 +980,7 @@
     </row>
     <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="9">
         <v>4</v>
@@ -969,63 +989,54 @@
         <v>22</v>
       </c>
       <c r="E21" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="9">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="9">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-    </row>
     <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="9">
+        <v>20</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="9">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C26" s="9">
         <v>20</v>
@@ -1034,12 +1045,12 @@
         <v>16</v>
       </c>
       <c r="E26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C27" s="9">
         <v>20</v>
@@ -1050,13 +1061,13 @@
       <c r="E27" s="2">
         <v>2</v>
       </c>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
     </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C28" s="9">
         <v>20</v>
@@ -1065,75 +1076,87 @@
         <v>16</v>
       </c>
       <c r="E28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="9">
-        <v>20</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
+        <v>3</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>15</v>
+        <v>67</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C30" s="9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E30" s="2">
-        <v>3</v>
-      </c>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="9">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C32" s="9">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="2">
         <v>1</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="F32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
     </row>
     <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C33" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E33" s="2">
         <v>0.3</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="G33"/>
       <c r="H33"/>
@@ -1141,7 +1164,10 @@
     </row>
     <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C34" s="9">
         <v>7</v>
@@ -1150,10 +1176,10 @@
         <v>27</v>
       </c>
       <c r="E34" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G34"/>
       <c r="H34"/>
@@ -1161,10 +1187,7 @@
     </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C35" s="9">
         <v>7</v>
@@ -1173,10 +1196,10 @@
         <v>27</v>
       </c>
       <c r="E35" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G35"/>
       <c r="H35"/>
@@ -1184,10 +1207,7 @@
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C36" s="9">
         <v>7</v>
@@ -1196,10 +1216,10 @@
         <v>27</v>
       </c>
       <c r="E36" s="2">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G36"/>
       <c r="H36"/>
@@ -1207,7 +1227,10 @@
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C37" s="9">
         <v>7</v>
@@ -1216,10 +1239,10 @@
         <v>27</v>
       </c>
       <c r="E37" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G37"/>
       <c r="H37"/>
@@ -1227,7 +1250,10 @@
     </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C38" s="9">
         <v>7</v>
@@ -1239,7 +1265,7 @@
         <v>5</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G38"/>
       <c r="H38"/>
@@ -1247,102 +1273,66 @@
     </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C39" s="9">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E39" s="2">
-        <v>2</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
     </row>
-    <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="9">
-        <v>7</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="2">
-        <v>5</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-    </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C41" s="9">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E41" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
     </row>
+    <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42"/>
+    </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="9">
-        <v>15</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
     </row>
     <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="9">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>66</v>
+      <c r="E44" s="7">
+        <f>SUM(E5:E43)</f>
+        <v>41.3</v>
       </c>
       <c r="G44"/>
     </row>
@@ -1350,23 +1340,13 @@
       <c r="G45"/>
     </row>
     <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="7">
-        <f>SUM(E5:E45)</f>
-        <v>42.3</v>
-      </c>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G49"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E41" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1409,7 +1389,7 @@
     </row>
     <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1417,7 +1397,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update scheduler demo to open AppEnd Settings component
Changed demoOpenScheduler in Dev_Scheduling.vue to open the BaseAppEndSettings component with updated title. Also updated ToDo.xlsx (binary changes).
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7819C063-EEC3-475A-BE78-A2E4E6BE2370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC0860F-D557-4740-86EA-0E2028124353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$39</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$47</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t>تسک</t>
   </si>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>ابزار چتباکس</t>
-  </si>
-  <si>
-    <t>CMS</t>
   </si>
   <si>
     <t>سایت فرانت آفیس</t>
@@ -675,11 +672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,354 +709,253 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="12">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="9">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="12">
-        <v>3</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="13">
-        <v>1</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="F8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C9" s="9">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C10" s="9">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="9">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2">
         <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C13" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="10">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="10">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="10"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="9">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="9">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
     </row>
     <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C20" s="9">
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E20" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C21" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="9">
-        <v>20</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="9">
-        <v>20</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="10"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="10"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="10"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C26" s="9">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E26" s="2">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
     </row>
     <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C27" s="9">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E27" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
@@ -1067,139 +963,106 @@
     </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C28" s="9">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
     </row>
+    <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="9">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+    </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="9">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C32" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C33" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E33" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C34" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C35" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E35" s="2">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="G35"/>
       <c r="H35"/>
@@ -1207,102 +1070,96 @@
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C36" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2">
-        <v>5</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
     </row>
-    <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="9">
-        <v>7</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="2">
-        <v>2</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-    </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C38" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E38" s="2">
-        <v>5</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C39" s="9">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="2">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
     </row>
+    <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="9">
+        <v>7</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+    </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>28</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C41" s="9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="E41" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G41"/>
       <c r="H41"/>
@@ -1310,43 +1167,189 @@
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="9">
+        <v>7</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="9">
+        <v>7</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="9">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="2">
+        <v>5</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="9">
+        <v>7</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="2">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="9">
+        <v>7</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="2">
+        <v>5</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="9">
+        <v>50</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+    </row>
+    <row r="49" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="9">
+        <v>15</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C50" s="9">
         <v>1</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E50" s="2">
         <v>0.5</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E44" s="7">
-        <f>SUM(E5:E43)</f>
-        <v>41.3</v>
-      </c>
-      <c r="G44"/>
-    </row>
-    <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G45"/>
-    </row>
-    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G46"/>
-    </row>
-    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G47"/>
+      <c r="F50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="7">
+        <f>SUM(E13:E51)</f>
+        <v>37.6</v>
+      </c>
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54"/>
+    </row>
+    <row r="55" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G55"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1389,7 +1392,7 @@
     </row>
     <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1397,7 +1400,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactor DB server handling to use proxy API
Migrated database server management from local state to model.DbServers and switched CRUD operations to Zzz.AppEndProxy methods. Simplified UI for DB servers, removed "Save All" functionality, and improved scheduled tasks layout. Cleaned up legacy code and moved LLM provider dropdown to toolbar.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC0860F-D557-4740-86EA-0E2028124353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7411CC9C-953A-4D7D-8137-1F4BE2D3EAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$47</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$43</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -672,11 +672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD18"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -856,159 +856,211 @@
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="9">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-    </row>
-    <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="9">
+      <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="9">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="10"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="10"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="9">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="9">
         <v>4</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2">
         <v>1</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="9">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="2">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="10"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="10"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="10"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="6"/>
+      <c r="F23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="9">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="9">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
     </row>
     <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="9">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="2">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="9">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-    </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C28" s="9">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C29" s="9">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E29" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="9">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="9">
+        <v>20</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C32" s="9">
         <v>20</v>
@@ -1017,52 +1069,44 @@
         <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="9">
-        <v>20</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="2">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
     </row>
     <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C34" s="9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E34" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C35" s="9">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E35" s="2">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="G35"/>
       <c r="H35"/>
@@ -1070,53 +1114,85 @@
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C36" s="9">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E36" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
     </row>
+    <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="9">
+        <v>7</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+    </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C38" s="9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E38" s="2">
-        <v>0.5</v>
-      </c>
+        <v>0.3</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
     </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C39" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E39" s="2">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="G39"/>
       <c r="H39"/>
@@ -1124,7 +1200,7 @@
     </row>
     <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C40" s="9">
         <v>7</v>
@@ -1133,7 +1209,7 @@
         <v>27</v>
       </c>
       <c r="E40" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>63</v>
@@ -1144,10 +1220,10 @@
     </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C41" s="9">
         <v>7</v>
@@ -1156,7 +1232,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>63</v>
@@ -1167,10 +1243,10 @@
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C42" s="9">
         <v>7</v>
@@ -1179,7 +1255,7 @@
         <v>27</v>
       </c>
       <c r="E42" s="2">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>63</v>
@@ -1190,59 +1266,33 @@
     </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C43" s="9">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="9">
-        <v>7</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="2">
-        <v>5</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-    </row>
     <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C45" s="9">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E45" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>63</v>
@@ -1253,103 +1303,43 @@
     </row>
     <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C46" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E46" s="2">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
     </row>
     <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="9">
-        <v>50</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" s="2">
-        <v>3</v>
-      </c>
       <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
-    </row>
-    <row r="49" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="9">
-        <v>15</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="2">
-        <v>1</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>63</v>
-      </c>
+    </row>
+    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="7">
+        <f>SUM(E13:E47)</f>
+        <v>37.6</v>
+      </c>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
-    </row>
-    <row r="50" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="9">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E50" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>63</v>
-      </c>
+    </row>
+    <row r="50" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G50"/>
     </row>
-    <row r="51" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G51"/>
     </row>
-    <row r="52" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E52" s="7">
-        <f>SUM(E13:E51)</f>
-        <v>37.6</v>
-      </c>
-      <c r="G52"/>
-    </row>
-    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G53"/>
-    </row>
-    <row r="54" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G54"/>
-    </row>
-    <row r="55" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G55"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E43" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor to use parameterized SQL for all DB calls
Replaced string interpolation with parameterized queries in both code generation (AppEndClass.cs) and generated repository (DefaultRepo.DbDirect.cs). Added helper methods to map C# types to SqlDbType and generate parameter lists. This improves security, type safety, and maintainability. Also updated ToDo.xlsx.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7411CC9C-953A-4D7D-8137-1F4BE2D3EAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8042DB38-8ABB-4179-AA9F-14530E9CBF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$43</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$45</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
   <si>
     <t>تسک</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>ابزارها و ..... - تزریق کانتکست</t>
+  </si>
+  <si>
+    <t>استفاده از گلوبال یوزینگ</t>
   </si>
 </sst>
 </file>
@@ -672,11 +675,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,257 +715,222 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C5" s="10">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E5" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C6" s="10">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E6" s="6">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="12">
-        <v>3</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C8" s="9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="12">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="13">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="9">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C10" s="9">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="9">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="9">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C15" s="9">
         <v>2</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E15" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C18" s="9">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E18" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C19" s="9">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E19" s="2">
         <v>2</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="6"/>
+      <c r="F19" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="2"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="9">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="2">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="9">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
+    <row r="22" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="10"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="10"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C24" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E24" s="2">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>63</v>
@@ -973,7 +941,7 @@
     </row>
     <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25" s="9">
         <v>4</v>
@@ -982,7 +950,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>63</v>
@@ -992,44 +960,53 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="9">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
     </row>
+    <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="9">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+    </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="9">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="9">
-        <v>20</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2</v>
-      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30" s="9">
         <v>20</v>
@@ -1038,12 +1015,12 @@
         <v>16</v>
       </c>
       <c r="E30" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C31" s="9">
         <v>20</v>
@@ -1054,13 +1031,13 @@
       <c r="E31" s="2">
         <v>2</v>
       </c>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C32" s="9">
         <v>20</v>
@@ -1069,87 +1046,75 @@
         <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>3</v>
-      </c>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="9">
+        <v>20</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
     </row>
     <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C34" s="9">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="9">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
+        <v>3</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="C36" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E36" s="2">
-        <v>1</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C37" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E37" s="2">
         <v>0.3</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G37"/>
       <c r="H37"/>
@@ -1157,10 +1122,7 @@
     </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C38" s="9">
         <v>7</v>
@@ -1169,7 +1131,7 @@
         <v>27</v>
       </c>
       <c r="E38" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>63</v>
@@ -1180,7 +1142,10 @@
     </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C39" s="9">
         <v>7</v>
@@ -1189,7 +1154,7 @@
         <v>27</v>
       </c>
       <c r="E39" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>63</v>
@@ -1200,7 +1165,10 @@
     </row>
     <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C40" s="9">
         <v>7</v>
@@ -1209,7 +1177,7 @@
         <v>27</v>
       </c>
       <c r="E40" s="2">
-        <v>5</v>
+        <v>0.3</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>63</v>
@@ -1220,10 +1188,7 @@
     </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C41" s="9">
         <v>7</v>
@@ -1232,7 +1197,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>63</v>
@@ -1243,10 +1208,7 @@
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C42" s="9">
         <v>7</v>
@@ -1266,80 +1228,126 @@
     </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C43" s="9">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E43" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
     </row>
+    <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="9">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="2">
+        <v>5</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+    </row>
     <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C45" s="9">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
     </row>
-    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="9">
+        <v>15</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C48" s="9">
         <v>1</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E48" s="2">
         <v>0.5</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G46"/>
-    </row>
-    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G47"/>
-    </row>
-    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E48" s="7">
-        <f>SUM(E13:E47)</f>
+      <c r="F48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="7">
+        <f>SUM(E15:E49)</f>
         <v>37.6</v>
       </c>
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G49"/>
-    </row>
-    <row r="50" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G50"/>
     </row>
-    <row r="51" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G51"/>
     </row>
+    <row r="52" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E43" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E45" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update .csproj to always copy server files to output
Refactored AppEndHost.csproj to explicitly mark key server-side .cs and .json files as content with CopyToOutputDirectory set to Always. This ensures all necessary code and configuration files are reliably copied to the output directory on every build. Also added Zzz.AppEndProxy.AAA.cs and updated Zzz.AppEndProxy.cs to always copy, improving deployment consistency.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8042DB38-8ABB-4179-AA9F-14530E9CBF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF02E4AB-52B2-4009-B4F9-17035D691808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$45</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$43</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>تسک</t>
   </si>
@@ -229,12 +229,6 @@
     <t>مثل کلاس DbDirrect</t>
   </si>
   <si>
-    <t>تکميل فرآیند DbDirect</t>
-  </si>
-  <si>
-    <t>اضافه کردن پارامترهای اوتپوت - صداکردن آبجکتها براساس پارامتر نه کانکت کردن ورودی ها</t>
-  </si>
-  <si>
     <t>ماسک برای اینپوتها</t>
   </si>
   <si>
@@ -284,9 +278,6 @@
   </si>
   <si>
     <t>ابزارها و ..... - تزریق کانتکست</t>
-  </si>
-  <si>
-    <t>استفاده از گلوبال یوزینگ</t>
   </si>
 </sst>
 </file>
@@ -675,11 +666,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,228 +703,246 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="10">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="10">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.5</v>
+      <c r="C7" s="12">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C8" s="9">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="12">
-        <v>3</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>63</v>
+      <c r="C9" s="9">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C10" s="9">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="9">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="9">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="2">
+    </row>
+    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="9">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="9">
+      <c r="F16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="9">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="2">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="9">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="9">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="F17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="10"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="2"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="10"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="10"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="6"/>
+    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="9">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="9">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
     </row>
     <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E24" s="2">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
@@ -941,7 +950,7 @@
     </row>
     <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="9">
         <v>4</v>
@@ -950,63 +959,54 @@
         <v>22</v>
       </c>
       <c r="E25" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="9">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="9">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-    </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="9">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="9">
+        <v>20</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C30" s="9">
         <v>20</v>
@@ -1015,12 +1015,12 @@
         <v>16</v>
       </c>
       <c r="E30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C31" s="9">
         <v>20</v>
@@ -1031,13 +1031,13 @@
       <c r="E31" s="2">
         <v>2</v>
       </c>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C32" s="9">
         <v>20</v>
@@ -1046,75 +1046,87 @@
         <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="9">
-        <v>20</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
+        <v>3</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
     </row>
     <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C34" s="9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E34" s="2">
-        <v>3</v>
-      </c>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="9">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C36" s="9">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="F36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C37" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E37" s="2">
         <v>0.3</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="G37"/>
       <c r="H37"/>
@@ -1122,7 +1134,10 @@
     </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C38" s="9">
         <v>7</v>
@@ -1131,10 +1146,10 @@
         <v>27</v>
       </c>
       <c r="E38" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G38"/>
       <c r="H38"/>
@@ -1142,10 +1157,7 @@
     </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C39" s="9">
         <v>7</v>
@@ -1154,10 +1166,10 @@
         <v>27</v>
       </c>
       <c r="E39" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G39"/>
       <c r="H39"/>
@@ -1165,10 +1177,7 @@
     </row>
     <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C40" s="9">
         <v>7</v>
@@ -1177,10 +1186,10 @@
         <v>27</v>
       </c>
       <c r="E40" s="2">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G40"/>
       <c r="H40"/>
@@ -1188,7 +1197,10 @@
     </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C41" s="9">
         <v>7</v>
@@ -1197,10 +1209,10 @@
         <v>27</v>
       </c>
       <c r="E41" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G41"/>
       <c r="H41"/>
@@ -1208,7 +1220,10 @@
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C42" s="9">
         <v>7</v>
@@ -1220,7 +1235,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G42"/>
       <c r="H42"/>
@@ -1228,126 +1243,80 @@
     </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C43" s="9">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E43" s="2">
-        <v>2</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="9">
-        <v>7</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="2">
-        <v>5</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-    </row>
     <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C45" s="9">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E45" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
     </row>
+    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G46"/>
+    </row>
     <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="9">
-        <v>15</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
     </row>
     <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="9">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>63</v>
+      <c r="E48" s="7">
+        <f>SUM(E13:E47)</f>
+        <v>37.6</v>
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G49"/>
     </row>
-    <row r="50" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="7">
-        <f>SUM(E15:E49)</f>
-        <v>37.6</v>
-      </c>
+    <row r="50" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G50"/>
     </row>
-    <row r="51" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G51"/>
     </row>
-    <row r="52" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G52"/>
-    </row>
-    <row r="53" spans="5:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G53"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E45" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E43" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1390,7 +1359,7 @@
     </row>
     <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1398,7 +1367,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add static/dynamic mode for RPC component generation
Added "Generate mode" dropdown to BaseRpcFunctionStudio.vue for static/dynamic component generation. Refactored code generation logic with buildDynamicCode and buildStaticCode methods. Static mode now produces explicit Vue components with form fields and output display. Improved generated component modal UI, switched to editable textarea, and enabled auto-maximize. Enhanced save logic to allow code editing before saving. Improved parameter parsing and input handling for static mode. Updated BaseRpcFunctionCaller.vue layout for split form/output mode. Minor UI and usability improvements. Updated ToDo.xlsx (binary change).
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF02E4AB-52B2-4009-B4F9-17035D691808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F28A6EB-1AEE-4BB0-9732-16E221C4E495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$43</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$54</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
   <si>
     <t>تسک</t>
   </si>
@@ -221,12 +221,6 @@
   </si>
   <si>
     <t>اکسپایری کلید - رفرش توکن</t>
-  </si>
-  <si>
-    <t>امکان تولید فرم روی فانکشنهایی که ورودی مستقیم دارند</t>
-  </si>
-  <si>
-    <t>مثل کلاس DbDirrect</t>
   </si>
   <si>
     <t>ماسک برای اینپوتها</t>
@@ -666,11 +660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -703,78 +697,127 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="10">
-        <v>10</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="6">
-        <v>0.5</v>
-      </c>
+      <c r="E4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="9">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C6" s="9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="12">
-        <v>3</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="9">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C8" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -782,308 +825,340 @@
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C9" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="9">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="9">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="9">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="12">
+        <v>3</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="13">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="9">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="9">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="9">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="10"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="6"/>
+      <c r="C21" s="9">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C22" s="9">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E22" s="2">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="9">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="9">
-        <v>4</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C25" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="12"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C28" s="9">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E28" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C29" s="9">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="E29" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="9">
-        <v>20</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="9">
-        <v>20</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="2">
-        <v>2</v>
-      </c>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="9">
-        <v>20</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="F29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="10"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="10"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="9">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="2">
         <v>3</v>
       </c>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="F33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
     </row>
     <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C34" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E34" s="2">
-        <v>0.5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
     </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C35" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E35" s="2">
-        <v>0.3</v>
+        <v>0.1</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="G35"/>
       <c r="H35"/>
@@ -1091,151 +1166,86 @@
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C36" s="9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E36" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="9">
-        <v>7</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
     </row>
-    <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="9">
-        <v>7</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-    </row>
     <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C39" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E39" s="2">
-        <v>1</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C40" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E40" s="2">
-        <v>5</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C41" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2">
-        <v>2</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C42" s="9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E42" s="2">
-        <v>5</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="G42"/>
       <c r="H42"/>
@@ -1243,13 +1253,13 @@
     </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C43" s="9">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E43" s="2">
         <v>3</v>
@@ -1260,63 +1270,269 @@
     </row>
     <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C45" s="9">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G45"/>
-      <c r="H45"/>
-      <c r="I45"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>52</v>
+        <v>23</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C46" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E46" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="9">
+        <v>7</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="9">
+        <v>7</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="9">
+        <v>7</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="9">
+        <v>7</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="9">
+        <v>7</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="2">
+        <v>5</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="9">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="9">
+        <v>7</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="2">
+        <v>5</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="9">
+        <v>50</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" s="2">
+        <v>3</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+    </row>
+    <row r="56" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="9">
+        <v>15</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="9">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="2">
         <v>0.5</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G46"/>
-    </row>
-    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G47"/>
-    </row>
-    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E48" s="7">
-        <f>SUM(E13:E47)</f>
+      <c r="F57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="7">
+        <f>SUM(E25:E58)</f>
         <v>37.6</v>
       </c>
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G49"/>
-    </row>
-    <row r="50" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G50"/>
-    </row>
-    <row r="51" spans="7:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G51"/>
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G60"/>
+    </row>
+    <row r="61" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G62"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E43" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E54" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1359,7 +1575,7 @@
     </row>
     <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1367,7 +1583,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactor: modularize jQuery plugins, add wizard dev guide
Split append-jQuery-plugins.js into modular plugin files and update bundle config. Add Dev_Wizard.vue as a comprehensive dev guide for bsTabsAutoNav, with live demos and documentation. Enhance bsTabsAutoNav with new stepper styles (connected-circles, arrow-steps, progress-bar) and improved navigation logic. Add detailed CSS for new steppers with RTL support. Remove legacy BaseWizard.vue and WizTest.vue. Update app.json to register the new dev guide. Modernizes wizard/stepper UX and improves maintainability.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD6F95-6ED0-4B9C-A7D9-FA1220EA85A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163A7A3E-DD8B-4AB5-B5C1-B7A2B4567ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$38</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$40</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>تسک</t>
   </si>
@@ -226,9 +226,6 @@
     <t>ماسک برای اینپوتها</t>
   </si>
   <si>
-    <t>بهینه سازی پلاگین ویزارد</t>
-  </si>
-  <si>
     <t>پلاگين</t>
   </si>
   <si>
@@ -272,6 +269,12 @@
   </si>
   <si>
     <t>ابزارها و ..... - تزریق کانتکست</t>
+  </si>
+  <si>
+    <t>پیاده سازی پرووایدر اوراکل</t>
+  </si>
+  <si>
+    <t>ماژول ریپورتینگ</t>
   </si>
 </sst>
 </file>
@@ -660,11 +663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -697,15 +700,15 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -745,13 +748,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -759,88 +762,34 @@
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C6" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2">
         <v>0.5</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8"/>
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="9">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" s="9">
         <v>7</v>
@@ -849,10 +798,10 @@
         <v>27</v>
       </c>
       <c r="E11" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -860,7 +809,10 @@
     </row>
     <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="9">
         <v>7</v>
@@ -869,10 +821,10 @@
         <v>27</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -880,7 +832,10 @@
     </row>
     <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="9">
         <v>7</v>
@@ -889,10 +844,10 @@
         <v>27</v>
       </c>
       <c r="E13" s="2">
-        <v>5</v>
+        <v>0.3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -900,10 +855,7 @@
     </row>
     <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="9">
         <v>7</v>
@@ -912,10 +864,10 @@
         <v>27</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -923,10 +875,7 @@
     </row>
     <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="9">
         <v>7</v>
@@ -938,223 +887,229 @@
         <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="9">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
     </row>
     <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C17" s="9">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
     </row>
+    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18"/>
+    </row>
     <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C19" s="9">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="12">
         <v>3</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="13">
-        <v>1</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
     </row>
     <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C21" s="9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="12">
+        <v>3</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="13">
         <v>1</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="9">
-        <v>10</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>59</v>
+      <c r="F22" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C23" s="9">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="9">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C25" s="9">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="9">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="10"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="9">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C28" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-    </row>
-    <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="9">
-        <v>4</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="10"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C30" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E30" s="2">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -1162,7 +1117,7 @@
     </row>
     <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C31" s="9">
         <v>4</v>
@@ -1171,49 +1126,58 @@
         <v>22</v>
       </c>
       <c r="E31" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
     </row>
+    <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="9">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
     <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C33" s="9">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E33" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="9">
-        <v>20</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="2">
-        <v>2</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
     </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C35" s="9">
         <v>20</v>
@@ -1222,12 +1186,12 @@
         <v>16</v>
       </c>
       <c r="E35" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C36" s="9">
         <v>20</v>
@@ -1238,13 +1202,13 @@
       <c r="E36" s="2">
         <v>2</v>
       </c>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C37" s="9">
         <v>20</v>
@@ -1253,33 +1217,70 @@
         <v>16</v>
       </c>
       <c r="E37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="9">
+        <v>20</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+    </row>
+    <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="9">
+        <v>20</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2">
         <v>3</v>
       </c>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-    </row>
-    <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G40"/>
-    </row>
-    <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="7">
-        <f>SUM(E7:E40)</f>
-        <v>39</v>
-      </c>
-      <c r="G41"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G42"/>
     </row>
     <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="7">
+        <f>SUM(E2:E42)</f>
+        <v>40</v>
+      </c>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G44"/>
     </row>
+    <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G46"/>
+    </row>
+    <row r="1048576" spans="5:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1048576" s="2">
+        <f>SUM(E3:E1048575)</f>
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E38" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1322,7 +1323,7 @@
     </row>
     <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1330,7 +1331,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add column-level access control for queries and UI
Implemented column access restrictions via new AccessDeny property in DbQueryColumn. Backend now filters columns based on denied users/roles before execution. Added JS helpers and updated UI templates to conditionally render or disable fields. Introduced DbDialogColAccessEditor.vue for editing access settings. Server now generates column access maps for client checks. Access control applies to both read and update scenarios. Minor code and UI improvements included.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163A7A3E-DD8B-4AB5-B5C1-B7A2B4567ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6449B032-8CA0-4E5D-9AB0-AF2F295E967D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$40</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>تسک</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>ماژول ریپورتینگ</t>
+  </si>
+  <si>
+    <t>وورک فلو انجین</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="A9:XFD9"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -785,6 +788,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="G10"/>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ToDo.xlsx with new spreadsheet data
The ToDo.xlsx file was modified, reflecting updates to its contents. This may include changes to tasks, statuses, or other spreadsheet data.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228E52FC-3E3F-4C94-89B5-43A92F895123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7070A6-AB6F-4611-8B65-0B383E25E042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="ماژول ها" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$39</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$40</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -663,16 +663,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1048575"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="94.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -703,58 +703,38 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>0.3</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -762,21 +742,36 @@
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -791,31 +786,11 @@
       <c r="G10"/>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="9">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
     </row>
     <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="9">
         <v>7</v>
@@ -824,7 +799,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>57</v>
@@ -835,10 +810,10 @@
     </row>
     <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="9">
         <v>7</v>
@@ -858,7 +833,10 @@
     </row>
     <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C14" s="9">
         <v>7</v>
@@ -867,7 +845,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>57</v>
@@ -878,7 +856,7 @@
     </row>
     <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="9">
         <v>7</v>
@@ -887,7 +865,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>57</v>
@@ -898,10 +876,7 @@
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="9">
         <v>7</v>
@@ -910,7 +885,7 @@
         <v>27</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>57</v>
@@ -921,10 +896,10 @@
     </row>
     <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9">
         <v>7</v>
@@ -933,7 +908,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>57</v>
@@ -943,173 +918,176 @@
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="9">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C20" s="9">
         <v>50</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <v>3</v>
       </c>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-    </row>
-    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C22" s="9">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E22" s="2">
         <v>0.5</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="F22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C23" s="12">
         <v>3</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E23" s="13">
         <v>1</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="9">
-        <v>10</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C24" s="9">
         <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="9">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="9">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="9">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C28" s="9">
         <v>5</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E28" s="2">
         <v>2</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="10"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="9">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="2">
-        <v>3</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
+      <c r="F28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="10"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C30" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E30" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>57</v>
@@ -1120,7 +1098,7 @@
     </row>
     <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" s="9">
         <v>4</v>
@@ -1129,7 +1107,7 @@
         <v>22</v>
       </c>
       <c r="E31" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>57</v>
@@ -1140,7 +1118,7 @@
     </row>
     <row r="32" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="9">
         <v>4</v>
@@ -1158,23 +1136,29 @@
       <c r="H32"/>
       <c r="I32"/>
     </row>
-    <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="9">
-        <v>20</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="2">
-        <v>2</v>
-      </c>
+    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="9">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
     </row>
     <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" s="9">
         <v>20</v>
@@ -1188,10 +1172,7 @@
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C36" s="9">
         <v>20</v>
@@ -1200,12 +1181,15 @@
         <v>16</v>
       </c>
       <c r="E36" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C37" s="9">
         <v>20</v>
@@ -1214,15 +1198,12 @@
         <v>16</v>
       </c>
       <c r="E37" s="2">
-        <v>2</v>
-      </c>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" s="9">
         <v>20</v>
@@ -1231,23 +1212,37 @@
         <v>16</v>
       </c>
       <c r="E38" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
     </row>
-    <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G41"/>
+    <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="9">
+        <v>20</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3</v>
+      </c>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
     </row>
     <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E42" s="7">
-        <f>SUM(E2:E41)</f>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="7">
+        <f>SUM(E2:E42)</f>
         <v>38.700000000000003</v>
       </c>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G43"/>
     </row>
     <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,14 +1251,17 @@
     <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G45"/>
     </row>
-    <row r="1048575" spans="5:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1048575" s="2">
-        <f>SUM(E3:E1048574)</f>
+    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G46"/>
+    </row>
+    <row r="1048576" spans="5:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1048576" s="2">
+        <f>SUM(E4:E1048575)</f>
         <v>77.400000000000006</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1271,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CBDBF2-162D-4D66-B456-CE5DDF1E2AB3}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1284,32 +1282,32 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -1317,10 +1315,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add workflow validation, diagnostics, and sample docs
Added SampleWorkflows.cs for workflow IDs/descriptions and usage notes. Introduced WorkflowSystemTest.cs for automated workflow system diagnostics and cache tests, callable via RPC. Implemented WorkflowValidator.cs to enforce schema validation on workflow JSON files. These changes improve reliability, testability, and documentation of the workflow system.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7070A6-AB6F-4611-8B65-0B383E25E042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA9A6B-B25D-4893-B4B3-5A378861D7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$40</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>تسک</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>تست</t>
+  </si>
+  <si>
+    <t>تمپلیت درخت</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -772,6 +775,11 @@
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add workflow management UI & RPC endpoints (WIP)
- Added "Workflow" section to app menu with manager, monitor, and tasks.
- Introduced Vue components for workflow CRUD, instance monitoring, and task handling.
- Refactored WorkflowServices.cs: new CRUD-style RPC endpoints for workflows and tasks, legacy Elsa code replaced/stubbed.
- Updated copilot-instructions.md with modal, loading, and list UI guidelines.
- Added RemoveFromCache() to WorkflowDefinitionProvider.
- Moved Zzz.AppEndProxy.*.cs files to <Compile> in csproj for runtime availability.
- Minor: updated ToDo.xlsx (binary change).
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA9A6B-B25D-4893-B4B3-5A378861D7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E4B224-DD85-43CD-9F49-4A76C5A207CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="بورد اصلی" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$40</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>تسک</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>تمپلیت درخت</t>
+  </si>
+  <si>
+    <t>ماژول مدیریت نود</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
@@ -1277,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CBDBF2-162D-4D66-B456-CE5DDF1E2AB3}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1336,6 +1339,11 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
+    <row r="9" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial release: Full Workflow Designer implementation
- Replaced placeholder with a complete visual workflow editor (WorkflowEditor.vue) featuring node palette, SVG canvas, and properties panel
- Added DesignerCanvas.vue for SVG-based node and connection rendering, drag-and-drop, and interactive editing
- Introduced workflowBuilder.js for workflow state, node/connection management, undo/redo, and validation logic
- Added nodeTypes.js defining 22 node types across 12 categories, with utility functions for palette and lookup
- Implemented workflow-designer.css for responsive, accessible, and animated UI styling
- Added WorkflowDesignerTest.vue for developer/QA testing of node types, categories, and validation
- Included comprehensive documentation: user/developer guides, changelog, summary, and architecture
- System is production-ready, extensible, and fully documented
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projects\AppEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E4B224-DD85-43CD-9F49-4A76C5A207CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E13478D-1727-4973-9ECA-78C1AC84DC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="بورد اصلی" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'بورد اصلی'!$A$1:$E$40</definedName>
-    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E311" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
+    <definedName name="_xlcn.WorksheetConnection_بورداصلیD1E31" hidden="1">'بورد اصلی'!$D$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E311"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_بورداصلیD1E31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -268,9 +268,6 @@
     <t>پیاده سازی پرووایدر اوراکل</t>
   </si>
   <si>
-    <t>ماژول ریپورتینگ</t>
-  </si>
-  <si>
     <t>وورک فلو انجین</t>
   </si>
   <si>
@@ -281,6 +278,9 @@
   </si>
   <si>
     <t>ماژول مدیریت نود</t>
+  </si>
+  <si>
+    <t>ماژول ریپورتینگ / داشبورد / وِژوالایزیشن</t>
   </si>
 </sst>
 </file>
@@ -671,9 +671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -714,7 +714,7 @@
         <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -782,17 +782,17 @@
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10"/>
     </row>
@@ -1282,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CBDBF2-162D-4D66-B456-CE5DDF1E2AB3}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="9" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>